<commit_message>
dalaila changed for lockdown item
</commit_message>
<xml_diff>
--- a/Dalaila Botique/2020/Dalaila2020.xlsx
+++ b/Dalaila Botique/2020/Dalaila2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pasal\Dalaila Botique\2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CCE847-F57E-4BC4-9D17-8EDBB8502ED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9440811-F6DE-46E6-8FE6-7AD86E2111ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1359,7 +1359,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###,###,###,###,##0.00"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1421,6 +1424,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ARIAL"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1442,7 +1451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1474,6 +1483,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3813,7 +3837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -5056,8 +5080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5165,101 +5189,143 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>207</v>
       </c>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>212</v>
       </c>
       <c r="C26" s="9"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="16">
+        <v>462</v>
+      </c>
+      <c r="E28" s="14">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="16">
+        <v>452</v>
+      </c>
+      <c r="E29" s="14">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="16">
+        <v>453</v>
+      </c>
+      <c r="E30" s="14">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>218</v>
+      </c>
+      <c r="C32" s="17">
+        <v>454</v>
+      </c>
+      <c r="E32" s="14">
+        <v>750</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>219</v>
       </c>
+      <c r="C33" s="17">
+        <v>455</v>
+      </c>
+      <c r="E33" s="14">
+        <v>2925</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>220</v>
       </c>
+      <c r="C34" s="17">
+        <v>456</v>
+      </c>
+      <c r="E34" s="14">
+        <v>705</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>221</v>
+      </c>
+      <c r="C35" s="17">
+        <v>457</v>
+      </c>
+      <c r="E35" s="14">
+        <v>550</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -5274,7 +5340,7 @@
       </c>
       <c r="E38" s="1">
         <f>SUM(E5:E36)</f>
-        <v>0</v>
+        <v>9182</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
@@ -5286,7 +5352,7 @@
       <c r="D40" s="12"/>
       <c r="E40" s="6">
         <f>SUM(D38:E38)</f>
-        <v>0</v>
+        <v>9182</v>
       </c>
     </row>
   </sheetData>
@@ -5304,10 +5370,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B1:L40"/>
+  <dimension ref="B1:O40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5318,7 +5384,7 @@
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5330,7 +5396,7 @@
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
     </row>
-    <row r="2" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="12" t="s">
         <v>384</v>
       </c>
@@ -5342,7 +5408,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" s="11" t="s">
         <v>375</v>
       </c>
@@ -5354,7 +5420,7 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>68</v>
       </c>
@@ -5364,64 +5430,105 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K4" s="18"/>
+      <c r="M4" s="14"/>
+      <c r="O4" s="15"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>458</v>
+      </c>
+      <c r="F5">
+        <v>852</v>
+      </c>
+      <c r="K5" s="18"/>
+      <c r="M5" s="14"/>
+      <c r="O5" s="15"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="18"/>
+      <c r="M6" s="14"/>
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>459</v>
+      </c>
+      <c r="F7">
+        <v>2267</v>
+      </c>
+      <c r="K7" s="18"/>
+      <c r="M7" s="14"/>
+      <c r="O7" s="15"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="18"/>
+      <c r="M8" s="14"/>
+      <c r="O8" s="15"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K9" s="18"/>
+      <c r="M9" s="14"/>
+      <c r="O9" s="15"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K10" s="18"/>
+      <c r="M10" s="14"/>
+      <c r="O10" s="15"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="18"/>
+      <c r="M11" s="14"/>
+      <c r="O11" s="15"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>462</v>
+      </c>
+      <c r="F15">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>233</v>
       </c>
@@ -5430,6 +5537,12 @@
       <c r="B17" t="s">
         <v>234</v>
       </c>
+      <c r="D17">
+        <v>463</v>
+      </c>
+      <c r="F17">
+        <v>3035</v>
+      </c>
       <c r="I17" t="s">
         <v>376</v>
       </c>
@@ -5453,11 +5566,23 @@
       <c r="B21" t="s">
         <v>238</v>
       </c>
+      <c r="D21">
+        <v>464</v>
+      </c>
+      <c r="F21">
+        <v>957</v>
+      </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>239</v>
       </c>
+      <c r="D22">
+        <v>465</v>
+      </c>
+      <c r="F22">
+        <v>3207</v>
+      </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -5468,6 +5593,12 @@
       <c r="B24" t="s">
         <v>241</v>
       </c>
+      <c r="D24">
+        <v>461</v>
+      </c>
+      <c r="F24">
+        <v>1495</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -5492,6 +5623,12 @@
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>246</v>
+      </c>
+      <c r="D29">
+        <v>460</v>
+      </c>
+      <c r="F29">
+        <v>490</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -5536,7 +5673,7 @@
       </c>
       <c r="F38" s="1">
         <f>SUM(F5:F36)</f>
-        <v>0</v>
+        <v>13063</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="1"/>
@@ -5551,7 +5688,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="6">
         <f>SUM(E38:F38)</f>
-        <v>0</v>
+        <v>13063</v>
       </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>

</xml_diff>